<commit_message>
:sparkles: Add lab04 files and description
</commit_message>
<xml_diff>
--- a/lab03/analiza_gva_porownanie_modeli_trendow.xlsx
+++ b/lab03/analiza_gva_porownanie_modeli_trendow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\.vscode\extensions\studia\time_series\lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65CADCF-1147-42FB-BAAB-85FCC35B7D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B347EF78-842F-4EFF-AE17-345FACE1547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2977F778-294C-41E8-84DB-D41E801134F5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{2977F778-294C-41E8-84DB-D41E801134F5}"/>
   </bookViews>
   <sheets>
     <sheet name="t.liniowy" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="t.logistyczny" sheetId="11" r:id="rId3"/>
     <sheet name="t.potegowy" sheetId="15" r:id="rId4"/>
     <sheet name="t.wykładniczy" sheetId="17" r:id="rId5"/>
-    <sheet name="t.potęgowy-analiza danych" sheetId="16" r:id="rId6"/>
-    <sheet name="t.wykładniczy-analiza danych" sheetId="18" r:id="rId7"/>
-    <sheet name="LOGARYTM NATURALNY OBLICZENIA" sheetId="3" r:id="rId8"/>
+    <sheet name="Gretl" sheetId="19" r:id="rId6"/>
+    <sheet name="t.potęgowy-analiza danych" sheetId="16" r:id="rId7"/>
+    <sheet name="t.wykładniczy-analiza danych" sheetId="18" r:id="rId8"/>
+    <sheet name="LOGARYTM NATURALNY OBLICZENIA" sheetId="3" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="2" hidden="1">t.logistyczny!$F$6:$F$8</definedName>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="101">
   <si>
     <t>Daty</t>
   </si>
@@ -330,10 +331,76 @@
     <t>Przeciętnie rzecz biorąc, z kwartału na kwartał gva rosła o 100,07 mln euro.</t>
   </si>
   <si>
-    <t>Średnio rzecz biorac, z kwartalu na kwartal gva rosła o 86,47 mln euro, co stanowi 0,2%  średniej kwartalnej GVA.</t>
+    <t>Średnio rzecz biorąc, z kwartału na kwartał, GVA rosła o 87,06 mln euro, co stanowi 0,21%  średniej kwartalnej GVA.</t>
   </si>
   <si>
-    <t>Średnio rzecz biorąc, z kwartału na kwartał, GVA rosła o 87,06 mln euro, co stanowi 0,21%  średniej kwartalnej GVA.</t>
+    <t>"Najlepszy" model trendu dla danych, tutaj kwadratowy.</t>
+  </si>
+  <si>
+    <t>Zweryfikowałem hipotezę głoszącą brak zmian strukturalnych w 2020,1 (covid).</t>
+  </si>
+  <si>
+    <t>Na 10% poziomie istotności należy odrzucić H0, zatem wnioskujemy o występowaniu załamania strukturalnego w okresie 2020,1.</t>
+  </si>
+  <si>
+    <t>Odrzucenie H0 wymaga redefiniowania modelu, tj. wprowadzenia zmiennych 0-1 pozwalających uwzględnić w modelu zmiany strukturalne.</t>
+  </si>
+  <si>
+    <t>Tworzymy zmienne przełącznikowe tj. 0-1.</t>
+  </si>
+  <si>
+    <t>Oszacowany model uwzględniający załamanie strukturalne w 2020,1</t>
+  </si>
+  <si>
+    <t>Wstępne wyniki wskazują na istotność wszystkich parametrów występujących przy zmiennych (d1, td1, sq_td1)</t>
+  </si>
+  <si>
+    <t>beta0</t>
+  </si>
+  <si>
+    <t>beta0_1</t>
+  </si>
+  <si>
+    <t>beta1</t>
+  </si>
+  <si>
+    <t>beta1_1</t>
+  </si>
+  <si>
+    <t>beta2</t>
+  </si>
+  <si>
+    <t>beta2_0</t>
+  </si>
+  <si>
+    <t>szybkość przed covidem</t>
+  </si>
+  <si>
+    <t>szybkość po covidzie</t>
+  </si>
+  <si>
+    <t>&lt;- średnia arytm. numerów obserwacji</t>
+  </si>
+  <si>
+    <t>tempo przed covidem</t>
+  </si>
+  <si>
+    <t>tempo po covidzie</t>
+  </si>
+  <si>
+    <t>średnia GVA w latach 2010-2019</t>
+  </si>
+  <si>
+    <t>średnia GVA w latach 2020,1 - 2025</t>
+  </si>
+  <si>
+    <t>średnia GVA przed Covid</t>
+  </si>
+  <si>
+    <t>średnia GVA od 2020</t>
+  </si>
+  <si>
+    <t>Średnio rzecz biorac, z kwartalu na kwartal gva rosła o 87,13 mln euro, co stanowi 0,21% średniej kwartalnej GVA.</t>
   </si>
 </sst>
 </file>
@@ -24754,6 +24821,275 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>248535</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>82488</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF981EEA-C4A7-8081-4AFC-F2E3AB535269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="182880"/>
+          <a:ext cx="6344535" cy="4105848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>162825</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>126365</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Obraz 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D992EC05-427E-3DDB-155C-2B6B12F5C1CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7124700" y="144780"/>
+          <a:ext cx="6449325" cy="4553585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>256193</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>113159</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Obraz 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45100F6C-1684-3EB8-B157-7FF22C4EFC19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="350520" y="4328160"/>
+          <a:ext cx="6611273" cy="5477639"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>92328</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>107334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Obraz 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CDE6BC4-A548-C5C9-4995-15A34A130EED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="434340" y="11879580"/>
+          <a:ext cx="6363588" cy="4686954"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>587644</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>149220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Obraz 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54741BBC-B454-5245-8B48-F517E6A6E91E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6911340" y="11910060"/>
+          <a:ext cx="6477904" cy="4515480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>21852</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>132074</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Obraz 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D09A04-05C1-E3D2-137B-8D8E36B87EC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="297180" y="16657320"/>
+          <a:ext cx="6430272" cy="4505954"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
@@ -25073,7 +25409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26911614-926A-4CE9-B376-543C75F0537F}">
   <dimension ref="A1:BM96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -28063,7 +28399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E572DCFF-398D-47B4-81B5-70BC65AC7419}">
   <dimension ref="A1:BN97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -32883,7 +33221,7 @@
         <v>87.056324444118445</v>
       </c>
       <c r="E90" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F90"/>
       <c r="G90"/>
@@ -33439,7 +33777,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59BC677-FF2E-4043-8227-BA4CCFA33C39}">
   <dimension ref="A1:P161"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -36330,7 +36670,7 @@
         <v>87.125402299536859</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="E72" s="15"/>
       <c r="F72" s="15"/>
@@ -37963,7 +38303,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5EDA4-8D45-479C-9CFE-88556DEDA72C}">
   <dimension ref="A1:BM95"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -40879,7 +41221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71526E28-90CB-4A6B-B997-5C265D9B5F2F}">
   <dimension ref="A1:BM95"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -43792,6 +44134,165 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD318CF-BC12-4366-B9E5-1505FC5EF53E}">
+  <dimension ref="M29:U110"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="T117" sqref="T117"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="29" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M93" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M94" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N98" t="s">
+        <v>85</v>
+      </c>
+      <c r="O98">
+        <v>50259.4</v>
+      </c>
+    </row>
+    <row r="99" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N99" t="s">
+        <v>86</v>
+      </c>
+      <c r="O99">
+        <v>-118175</v>
+      </c>
+      <c r="R99" t="s">
+        <v>98</v>
+      </c>
+      <c r="T99">
+        <v>40785.14499999999</v>
+      </c>
+    </row>
+    <row r="100" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N100" t="s">
+        <v>87</v>
+      </c>
+      <c r="O100">
+        <v>-979.66099999999994</v>
+      </c>
+      <c r="R100" t="s">
+        <v>99</v>
+      </c>
+      <c r="T100">
+        <v>45260.577272727278</v>
+      </c>
+    </row>
+    <row r="101" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N101" t="s">
+        <v>88</v>
+      </c>
+      <c r="O101">
+        <v>4520.09</v>
+      </c>
+    </row>
+    <row r="102" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N102" t="s">
+        <v>89</v>
+      </c>
+      <c r="O102">
+        <v>19.166799999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N103" t="s">
+        <v>90</v>
+      </c>
+      <c r="O103">
+        <v>-44.851599999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="Q105">
+        <v>20.5</v>
+      </c>
+      <c r="S105">
+        <v>51.5</v>
+      </c>
+      <c r="U105" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="106" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N106" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q106">
+        <f>O100+(2*O102*20.5)</f>
+        <v>-193.82219999999995</v>
+      </c>
+    </row>
+    <row r="107" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N107" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q107">
+        <f>(O100+O101)+(2*(O102+O103)*51.5)</f>
+        <v>894.89460000000008</v>
+      </c>
+    </row>
+    <row r="109" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N109" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q109" s="32">
+        <f>Q106/T99</f>
+        <v>-4.7522743881381318E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="14:21" x14ac:dyDescent="0.3">
+      <c r="N110" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q110" s="32">
+        <f>Q107/T100</f>
+        <v>1.9772054488117141E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2D47CF-CC83-4181-9730-3C41A292D8EA}">
   <dimension ref="A1:I18"/>
   <sheetViews>
@@ -44013,7 +44514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65824C5-3561-4E84-B29D-52299CB24F42}">
   <dimension ref="A1:I18"/>
   <sheetViews>
@@ -44235,11 +44736,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBBEA22-52AA-419A-9E86-6CF5CEEAF39E}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -44250,7 +44753,7 @@
     <col min="5" max="28" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -44267,7 +44770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2010.1</v>
       </c>
@@ -44285,8 +44788,11 @@
         <f>LN(D2)</f>
         <v>0.69314718055994529</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2010.2</v>
       </c>
@@ -44304,8 +44810,11 @@
         <f t="shared" ref="E3:E63" si="1">LN(D3)</f>
         <v>1.0986122886681098</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2010.3</v>
       </c>
@@ -44323,8 +44832,11 @@
         <f t="shared" si="1"/>
         <v>1.3862943611198906</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2010.4</v>
       </c>
@@ -44342,8 +44854,11 @@
         <f t="shared" si="1"/>
         <v>1.6094379124341003</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2011.1</v>
       </c>
@@ -44361,8 +44876,11 @@
         <f t="shared" si="1"/>
         <v>1.791759469228055</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2011.2</v>
       </c>
@@ -44380,8 +44898,11 @@
         <f t="shared" si="1"/>
         <v>1.9459101490553132</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2011.3</v>
       </c>
@@ -44399,8 +44920,11 @@
         <f t="shared" si="1"/>
         <v>2.0794415416798357</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2011.4</v>
       </c>
@@ -44418,8 +44942,11 @@
         <f t="shared" si="1"/>
         <v>2.1972245773362196</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2012.1</v>
       </c>
@@ -44437,8 +44964,11 @@
         <f t="shared" si="1"/>
         <v>2.3025850929940459</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2012.2</v>
       </c>
@@ -44456,8 +44986,11 @@
         <f t="shared" si="1"/>
         <v>2.3978952727983707</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2012.3</v>
       </c>
@@ -44475,8 +45008,11 @@
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2012.4</v>
       </c>
@@ -44494,8 +45030,11 @@
         <f t="shared" si="1"/>
         <v>2.5649493574615367</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2013.1</v>
       </c>
@@ -44513,8 +45052,11 @@
         <f t="shared" si="1"/>
         <v>2.6390573296152584</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2013.2</v>
       </c>
@@ -44532,8 +45074,11 @@
         <f t="shared" si="1"/>
         <v>2.7080502011022101</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2013.3</v>
       </c>
@@ -44551,8 +45096,11 @@
         <f t="shared" si="1"/>
         <v>2.7725887222397811</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2013.4</v>
       </c>
@@ -44570,8 +45118,11 @@
         <f t="shared" si="1"/>
         <v>2.8332133440562162</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2014.1</v>
       </c>
@@ -44589,8 +45140,11 @@
         <f t="shared" si="1"/>
         <v>2.8903717578961645</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2014.2</v>
       </c>
@@ -44608,8 +45162,11 @@
         <f t="shared" si="1"/>
         <v>2.9444389791664403</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2014.3</v>
       </c>
@@ -44627,8 +45184,11 @@
         <f t="shared" si="1"/>
         <v>2.9957322735539909</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2014.4</v>
       </c>
@@ -44646,8 +45206,11 @@
         <f t="shared" si="1"/>
         <v>3.044522437723423</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2015.1</v>
       </c>
@@ -44665,8 +45228,11 @@
         <f t="shared" si="1"/>
         <v>3.0910424533583161</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2015.2</v>
       </c>
@@ -44684,8 +45250,11 @@
         <f t="shared" si="1"/>
         <v>3.1354942159291497</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2015.3</v>
       </c>
@@ -44703,8 +45272,11 @@
         <f t="shared" si="1"/>
         <v>3.1780538303479458</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2015.4</v>
       </c>
@@ -44722,8 +45294,11 @@
         <f t="shared" si="1"/>
         <v>3.2188758248682006</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2016.1</v>
       </c>
@@ -44741,8 +45316,11 @@
         <f t="shared" si="1"/>
         <v>3.2580965380214821</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2016.2</v>
       </c>
@@ -44760,8 +45338,11 @@
         <f t="shared" si="1"/>
         <v>3.2958368660043291</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2016.3</v>
       </c>
@@ -44779,8 +45360,11 @@
         <f t="shared" si="1"/>
         <v>3.3322045101752038</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2016.4</v>
       </c>
@@ -44798,8 +45382,11 @@
         <f t="shared" si="1"/>
         <v>3.3672958299864741</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2017.1</v>
       </c>
@@ -44817,8 +45404,11 @@
         <f t="shared" si="1"/>
         <v>3.4011973816621555</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2017.2</v>
       </c>
@@ -44836,8 +45426,11 @@
         <f t="shared" si="1"/>
         <v>3.4339872044851463</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2017.3</v>
       </c>
@@ -44855,8 +45448,11 @@
         <f t="shared" si="1"/>
         <v>3.4657359027997265</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2017.4</v>
       </c>
@@ -44874,8 +45470,11 @@
         <f t="shared" si="1"/>
         <v>3.4965075614664802</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2018.1</v>
       </c>
@@ -44893,8 +45492,11 @@
         <f t="shared" si="1"/>
         <v>3.5263605246161616</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2018.2</v>
       </c>
@@ -44912,8 +45514,11 @@
         <f t="shared" si="1"/>
         <v>3.5553480614894135</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2018.3</v>
       </c>
@@ -44931,8 +45536,11 @@
         <f t="shared" si="1"/>
         <v>3.5835189384561099</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2018.4</v>
       </c>
@@ -44950,8 +45558,11 @@
         <f t="shared" si="1"/>
         <v>3.6109179126442243</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2019.1</v>
       </c>
@@ -44969,8 +45580,11 @@
         <f t="shared" si="1"/>
         <v>3.6375861597263857</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2019.2</v>
       </c>
@@ -44988,8 +45602,11 @@
         <f t="shared" si="1"/>
         <v>3.6635616461296463</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2019.3</v>
       </c>
@@ -45007,8 +45624,11 @@
         <f t="shared" si="1"/>
         <v>3.6888794541139363</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2019.4</v>
       </c>
@@ -45026,8 +45646,15 @@
         <f t="shared" si="1"/>
         <v>3.713572066704308</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <v>40</v>
+      </c>
+      <c r="I41">
+        <f>AVERAGEA(G2:G41)</f>
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2020.1</v>
       </c>
@@ -45045,8 +45672,11 @@
         <f t="shared" si="1"/>
         <v>3.7376696182833684</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2020.2</v>
       </c>
@@ -45064,8 +45694,15 @@
         <f t="shared" si="1"/>
         <v>3.7612001156935624</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>42</v>
+      </c>
+      <c r="I43">
+        <f>AVERAGEA(G42:G63)</f>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2020.3</v>
       </c>
@@ -45083,8 +45720,11 @@
         <f t="shared" si="1"/>
         <v>3.784189633918261</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2020.4</v>
       </c>
@@ -45102,8 +45742,11 @@
         <f t="shared" si="1"/>
         <v>3.8066624897703196</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2021.1</v>
       </c>
@@ -45121,8 +45764,11 @@
         <f t="shared" si="1"/>
         <v>3.8286413964890951</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2021.2</v>
       </c>
@@ -45140,8 +45786,11 @@
         <f t="shared" si="1"/>
         <v>3.8501476017100584</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2021.3</v>
       </c>
@@ -45159,8 +45808,11 @@
         <f t="shared" si="1"/>
         <v>3.8712010109078911</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2021.4</v>
       </c>
@@ -45178,8 +45830,11 @@
         <f t="shared" si="1"/>
         <v>3.8918202981106265</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2022.1</v>
       </c>
@@ -45197,8 +45852,11 @@
         <f t="shared" si="1"/>
         <v>3.912023005428146</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2022.2</v>
       </c>
@@ -45216,8 +45874,11 @@
         <f t="shared" si="1"/>
         <v>3.9318256327243257</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2022.3</v>
       </c>
@@ -45235,8 +45896,11 @@
         <f t="shared" si="1"/>
         <v>3.9512437185814275</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2022.4</v>
       </c>
@@ -45254,8 +45918,11 @@
         <f t="shared" si="1"/>
         <v>3.970291913552122</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2023.1</v>
       </c>
@@ -45273,8 +45940,11 @@
         <f t="shared" si="1"/>
         <v>3.9889840465642745</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2023.2</v>
       </c>
@@ -45292,8 +45962,11 @@
         <f t="shared" si="1"/>
         <v>4.0073331852324712</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2023.3</v>
       </c>
@@ -45311,8 +45984,11 @@
         <f t="shared" si="1"/>
         <v>4.0253516907351496</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2023.4</v>
       </c>
@@ -45330,8 +46006,11 @@
         <f t="shared" si="1"/>
         <v>4.0430512678345503</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2024.1</v>
       </c>
@@ -45349,8 +46028,11 @@
         <f t="shared" si="1"/>
         <v>4.0604430105464191</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2024.2</v>
       </c>
@@ -45368,8 +46050,11 @@
         <f t="shared" si="1"/>
         <v>4.0775374439057197</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2024.3</v>
       </c>
@@ -45387,8 +46072,11 @@
         <f t="shared" si="1"/>
         <v>4.0943445622221004</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2024.4</v>
       </c>
@@ -45406,8 +46094,11 @@
         <f t="shared" si="1"/>
         <v>4.1108738641733114</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2025.1</v>
       </c>
@@ -45425,8 +46116,11 @@
         <f t="shared" si="1"/>
         <v>4.1271343850450917</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2025.2</v>
       </c>
@@ -45444,17 +46138,36 @@
         <f t="shared" si="1"/>
         <v>4.1431347263915326</v>
       </c>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66" s="1">
+        <f>AVERAGE(B2:B41)</f>
+        <v>40785.14499999999</v>
+      </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>97</v>
+      </c>
+      <c r="E67" s="1">
+        <f>AVERAGE(B42:B63)</f>
+        <v>45260.577272727278</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45470,6 +46183,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AA02DD375EACAC4FB15EEC8FD8FFC49B" ma:contentTypeVersion="15" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="f277efaaccb9604b371bfb34b8a7b02d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df20a811-f17a-454b-a878-f104ad76a41c" xmlns:ns4="e4643e21-c9d5-45ab-a099-62e58f861c93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1023a9ed3908abd5cf15810256093846" ns3:_="" ns4:_="">
     <xsd:import namespace="df20a811-f17a-454b-a878-f104ad76a41c"/>
@@ -45704,15 +46426,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{388DA980-E041-4F9A-8DF2-47093692E34E}">
   <ds:schemaRefs>
@@ -45731,6 +46444,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75F1182F-CAF4-4608-99A5-03B2E59145BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B400A54C-1C51-4C97-BB2B-D8041266627C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45747,12 +46468,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75F1182F-CAF4-4608-99A5-03B2E59145BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>